<commit_message>
revisi commit kesembilan david
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Scrummaster" sheetId="3" r:id="rId1"/>
+    <sheet name="Initial" sheetId="4" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Done :</t>
   </si>
@@ -50,13 +50,79 @@
   </si>
   <si>
     <t>Penjelasan pada Sprint 1</t>
+  </si>
+  <si>
+    <t>1. Pengertian Software</t>
+  </si>
+  <si>
+    <t>2. Pengertian Hardware</t>
+  </si>
+  <si>
+    <t>3. Pengertian Brainware</t>
+  </si>
+  <si>
+    <t>4. Contoh Hardware</t>
+  </si>
+  <si>
+    <t>5. Contoh Software</t>
+  </si>
+  <si>
+    <t>6. Contoh Brainware</t>
+  </si>
+  <si>
+    <t>7. Index</t>
+  </si>
+  <si>
+    <t>8. Menu</t>
+  </si>
+  <si>
+    <t>Penjelasan Tahapan Sebelum Memulai Proyek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 1 : </t>
+  </si>
+  <si>
+    <t>(3 hari)</t>
+  </si>
+  <si>
+    <t>Sprint 2 :</t>
+  </si>
+  <si>
+    <t>Sprint 3 :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 4 : </t>
+  </si>
+  <si>
+    <t>Sprint 5 :</t>
+  </si>
+  <si>
+    <t>David Tjin</t>
+  </si>
+  <si>
+    <t>Albert Wijaya</t>
+  </si>
+  <si>
+    <t>Ismail Gohzali</t>
+  </si>
+  <si>
+    <t>Ricky Wijaya</t>
+  </si>
+  <si>
+    <t>(4 hari)</t>
+  </si>
+  <si>
+    <t>(1 harI)</t>
+  </si>
+  <si>
+    <t>Scrummaster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +137,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -94,11 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,14 +193,63 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>179902</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="838200"/>
+          <a:ext cx="10058400" cy="4485202"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>78082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -449,37 +573,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:S39"/>
+  <dimension ref="C2:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U28" sqref="U27:V28"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
+    <row r="2" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -497,79 +602,294 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>1</v>
-      </c>
-      <c r="K34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>3</v>
-      </c>
-      <c r="K36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="K37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K39" t="s">
-        <v>9</v>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:S2"/>
+    <mergeCell ref="C2:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:S38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S4" sqref="C4:S4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:S3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:S37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:S3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="K33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:S3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>